<commit_message>
GraphWorkspace: after refreshing selected dataframe → automatically reflect the properties of selected graph in GUI
</commit_message>
<xml_diff>
--- a/examples/data_inline.xlsx
+++ b/examples/data_inline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VL251876\Documents\Python\SPECTROview-1\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B38FB2F3-3BBB-4F70-B53C-9BE63C47DB76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C119CD41-17A7-4967-B8AC-623A168F988D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43035" yWindow="1755" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
@@ -529,8 +529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O589"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23793,8 +23793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D4DAA12-D9A6-4C89-A6AF-803390C58A71}">
   <dimension ref="A1:N589"/>
   <sheetViews>
-    <sheetView topLeftCell="A232" workbookViewId="0">
-      <selection activeCell="H318" sqref="H318:K327"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23839,7 +23839,7 @@
       <c r="M1" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="N1" s="10"/>
+      <c r="N1" s="8"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="3">

</xml_diff>